<commit_message>
Fix mistake in trial names
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\iwccla\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18210" windowHeight="10275" activeTab="1"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="input" sheetId="3" r:id="rId3"/>
     <sheet name="info" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1214,7 +1219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1971,9 +1976,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2134,7 @@
         <v>R1</v>
       </c>
       <c r="W2" s="6" t="str">
-        <f>IF(AND(B2=0,E2=1),"F1",IF(AND(B2=0,E2=2),"F2",IF(AND(B2=1,E2=1),"M1",IF(AND(B2=1,E2=2),"F2","?"))))</f>
+        <f>IF(AND(B2=0,E2=1),"F1",IF(AND(B2=0,E2=2),"F2",IF(AND(B2=1,E2=1),"M1",IF(AND(B2=1,E2=2),"M2","?"))))</f>
         <v>F1</v>
       </c>
       <c r="X2" s="6" t="str">
@@ -2207,7 +2212,7 @@
         <v>S1</v>
       </c>
       <c r="W3" s="6" t="str">
-        <f t="shared" ref="W3:W66" si="1">IF(AND(B3=0,E3=1),"F1",IF(AND(B3=0,E3=2),"F2",IF(AND(B3=1,E3=1),"M1",IF(AND(B3=1,E3=2),"F2","?"))))</f>
+        <f t="shared" ref="W3:W66" si="1">IF(AND(B3=0,E3=1),"F1",IF(AND(B3=0,E3=2),"F2",IF(AND(B3=1,E3=1),"M1",IF(AND(B3=1,E3=2),"M2","?"))))</f>
         <v>F1</v>
       </c>
       <c r="X3" s="6" t="str">
@@ -3534,11 +3539,11 @@
       </c>
       <c r="W20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-R1</v>
+        <v>M2-T1-R1</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -3612,11 +3617,11 @@
       </c>
       <c r="W21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X21" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-S1</v>
+        <v>M2-T1-S1</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -3690,11 +3695,11 @@
       </c>
       <c r="W22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-D1</v>
+        <v>M2-T1-D1</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -3768,11 +3773,11 @@
       </c>
       <c r="W23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X23" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-R4</v>
+        <v>M2-T1-R4</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -3846,11 +3851,11 @@
       </c>
       <c r="W24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-S4</v>
+        <v>M2-T1-S4</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -3924,11 +3929,11 @@
       </c>
       <c r="W25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X25" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T1-D4</v>
+        <v>M2-T1-D4</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -5406,11 +5411,11 @@
       </c>
       <c r="W44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X44" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-R1</v>
+        <v>M2-T2-R1</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
@@ -5484,11 +5489,11 @@
       </c>
       <c r="W45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X45" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-S1</v>
+        <v>M2-T2-S1</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
@@ -5562,11 +5567,11 @@
       </c>
       <c r="W46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X46" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-D1</v>
+        <v>M2-T2-D1</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -5640,11 +5645,11 @@
       </c>
       <c r="W47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X47" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-R4</v>
+        <v>M2-T2-R4</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -5718,11 +5723,11 @@
       </c>
       <c r="W48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X48" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-S4</v>
+        <v>M2-T2-S4</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -5796,11 +5801,11 @@
       </c>
       <c r="W49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X49" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>F2-T2-D4</v>
+        <v>M2-T2-D4</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
@@ -7199,7 +7204,7 @@
         <v>D4</v>
       </c>
       <c r="W67" s="3" t="str">
-        <f t="shared" ref="W67:W130" si="4">IF(AND(B67=0,E67=1),"F1",IF(AND(B67=0,E67=2),"F2",IF(AND(B67=1,E67=1),"M1",IF(AND(B67=1,E67=2),"F2","?"))))</f>
+        <f t="shared" ref="W67:W130" si="4">IF(AND(B67=0,E67=1),"F1",IF(AND(B67=0,E67=2),"F2",IF(AND(B67=1,E67=1),"M1",IF(AND(B67=1,E67=2),"M2","?"))))</f>
         <v>M1</v>
       </c>
       <c r="X67" s="3" t="str">
@@ -7278,11 +7283,11 @@
       </c>
       <c r="W68" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X68" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-R1</v>
+        <v>M2-T3-R1</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
@@ -7356,11 +7361,11 @@
       </c>
       <c r="W69" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X69" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-S1</v>
+        <v>M2-T3-S1</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
@@ -7434,11 +7439,11 @@
       </c>
       <c r="W70" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X70" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-D1</v>
+        <v>M2-T3-D1</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
@@ -7512,11 +7517,11 @@
       </c>
       <c r="W71" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X71" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-R4</v>
+        <v>M2-T3-R4</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
@@ -7590,11 +7595,11 @@
       </c>
       <c r="W72" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X72" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-S4</v>
+        <v>M2-T3-S4</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -7668,11 +7673,11 @@
       </c>
       <c r="W73" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X73" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T3-D4</v>
+        <v>M2-T3-D4</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
@@ -9150,11 +9155,11 @@
       </c>
       <c r="W92" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X92" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-R1</v>
+        <v>M2-T5-R1</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
@@ -9228,11 +9233,11 @@
       </c>
       <c r="W93" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X93" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-S1</v>
+        <v>M2-T5-S1</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.25">
@@ -9306,11 +9311,11 @@
       </c>
       <c r="W94" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X94" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-D1</v>
+        <v>M2-T5-D1</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
@@ -9384,11 +9389,11 @@
       </c>
       <c r="W95" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X95" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-R4</v>
+        <v>M2-T5-R4</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
@@ -9462,11 +9467,11 @@
       </c>
       <c r="W96" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X96" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-S4</v>
+        <v>M2-T5-S4</v>
       </c>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
@@ -9540,11 +9545,11 @@
       </c>
       <c r="W97" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X97" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T5-D4</v>
+        <v>M2-T5-D4</v>
       </c>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
@@ -11022,11 +11027,11 @@
       </c>
       <c r="W116" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X116" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-R1</v>
+        <v>M2-T10A-R1</v>
       </c>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
@@ -11100,11 +11105,11 @@
       </c>
       <c r="W117" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X117" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-S1</v>
+        <v>M2-T10A-S1</v>
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
@@ -11178,11 +11183,11 @@
       </c>
       <c r="W118" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X118" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-D1</v>
+        <v>M2-T10A-D1</v>
       </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
@@ -11256,11 +11261,11 @@
       </c>
       <c r="W119" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X119" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-R4</v>
+        <v>M2-T10A-R4</v>
       </c>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
@@ -11334,11 +11339,11 @@
       </c>
       <c r="W120" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X120" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-S4</v>
+        <v>M2-T10A-S4</v>
       </c>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
@@ -11412,11 +11417,11 @@
       </c>
       <c r="W121" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X121" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>F2-T10A-D4</v>
+        <v>M2-T10A-D4</v>
       </c>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
@@ -12191,7 +12196,7 @@
         <v>R4</v>
       </c>
       <c r="W131" s="3" t="str">
-        <f t="shared" ref="W131:W194" si="7">IF(AND(B131=0,E131=1),"F1",IF(AND(B131=0,E131=2),"F2",IF(AND(B131=1,E131=1),"M1",IF(AND(B131=1,E131=2),"F2","?"))))</f>
+        <f t="shared" ref="W131:W194" si="7">IF(AND(B131=0,E131=1),"F1",IF(AND(B131=0,E131=2),"F2",IF(AND(B131=1,E131=1),"M1",IF(AND(B131=1,E131=2),"M2","?"))))</f>
         <v>F2</v>
       </c>
       <c r="X131" s="3" t="str">
@@ -12894,11 +12899,11 @@
       </c>
       <c r="W140" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X140" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-R1</v>
+        <v>M2-T11A-R1</v>
       </c>
     </row>
     <row r="141" spans="1:24" x14ac:dyDescent="0.25">
@@ -12972,11 +12977,11 @@
       </c>
       <c r="W141" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X141" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-S1</v>
+        <v>M2-T11A-S1</v>
       </c>
     </row>
     <row r="142" spans="1:24" x14ac:dyDescent="0.25">
@@ -13050,11 +13055,11 @@
       </c>
       <c r="W142" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X142" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-D1</v>
+        <v>M2-T11A-D1</v>
       </c>
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
@@ -13128,11 +13133,11 @@
       </c>
       <c r="W143" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X143" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-R4</v>
+        <v>M2-T11A-R4</v>
       </c>
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
@@ -13206,11 +13211,11 @@
       </c>
       <c r="W144" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X144" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-S4</v>
+        <v>M2-T11A-S4</v>
       </c>
     </row>
     <row r="145" spans="1:24" x14ac:dyDescent="0.25">
@@ -13284,11 +13289,11 @@
       </c>
       <c r="W145" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X145" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T11A-D4</v>
+        <v>M2-T11A-D4</v>
       </c>
     </row>
     <row r="146" spans="1:24" x14ac:dyDescent="0.25">
@@ -14766,11 +14771,11 @@
       </c>
       <c r="W164" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X164" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-R1</v>
+        <v>M2-T12B-R1</v>
       </c>
     </row>
     <row r="165" spans="1:24" x14ac:dyDescent="0.25">
@@ -14844,11 +14849,11 @@
       </c>
       <c r="W165" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X165" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-S1</v>
+        <v>M2-T12B-S1</v>
       </c>
     </row>
     <row r="166" spans="1:24" x14ac:dyDescent="0.25">
@@ -14922,11 +14927,11 @@
       </c>
       <c r="W166" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X166" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-D1</v>
+        <v>M2-T12B-D1</v>
       </c>
     </row>
     <row r="167" spans="1:24" x14ac:dyDescent="0.25">
@@ -15000,11 +15005,11 @@
       </c>
       <c r="W167" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X167" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-R4</v>
+        <v>M2-T12B-R4</v>
       </c>
     </row>
     <row r="168" spans="1:24" x14ac:dyDescent="0.25">
@@ -15078,11 +15083,11 @@
       </c>
       <c r="W168" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X168" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-S4</v>
+        <v>M2-T12B-S4</v>
       </c>
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.25">
@@ -15156,11 +15161,11 @@
       </c>
       <c r="W169" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X169" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12B-D4</v>
+        <v>M2-T12B-D4</v>
       </c>
     </row>
     <row r="170" spans="1:24" x14ac:dyDescent="0.25">
@@ -16638,11 +16643,11 @@
       </c>
       <c r="W188" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X188" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-R1</v>
+        <v>M2-T12A-R1</v>
       </c>
     </row>
     <row r="189" spans="1:24" x14ac:dyDescent="0.25">
@@ -16716,11 +16721,11 @@
       </c>
       <c r="W189" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X189" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-S1</v>
+        <v>M2-T12A-S1</v>
       </c>
     </row>
     <row r="190" spans="1:24" x14ac:dyDescent="0.25">
@@ -16794,11 +16799,11 @@
       </c>
       <c r="W190" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X190" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-D1</v>
+        <v>M2-T12A-D1</v>
       </c>
     </row>
     <row r="191" spans="1:24" x14ac:dyDescent="0.25">
@@ -16872,11 +16877,11 @@
       </c>
       <c r="W191" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X191" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-R4</v>
+        <v>M2-T12A-R4</v>
       </c>
     </row>
     <row r="192" spans="1:24" x14ac:dyDescent="0.25">
@@ -16950,11 +16955,11 @@
       </c>
       <c r="W192" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X192" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-S4</v>
+        <v>M2-T12A-S4</v>
       </c>
     </row>
     <row r="193" spans="1:24" x14ac:dyDescent="0.25">
@@ -17028,11 +17033,11 @@
       </c>
       <c r="W193" s="3" t="str">
         <f t="shared" si="7"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X193" s="3" t="str">
         <f t="shared" si="8"/>
-        <v>F2-T12A-D4</v>
+        <v>M2-T12A-D4</v>
       </c>
     </row>
     <row r="194" spans="1:24" x14ac:dyDescent="0.25">
@@ -17183,7 +17188,7 @@
         <v>?</v>
       </c>
       <c r="W195" s="3" t="str">
-        <f t="shared" ref="W195:W258" si="10">IF(AND(B195=0,E195=1),"F1",IF(AND(B195=0,E195=2),"F2",IF(AND(B195=1,E195=1),"M1",IF(AND(B195=1,E195=2),"F2","?"))))</f>
+        <f t="shared" ref="W195:W258" si="10">IF(AND(B195=0,E195=1),"F1",IF(AND(B195=0,E195=2),"F2",IF(AND(B195=1,E195=1),"M1",IF(AND(B195=1,E195=2),"M2","?"))))</f>
         <v>F1</v>
       </c>
       <c r="X195" s="3" t="str">
@@ -17574,11 +17579,11 @@
       </c>
       <c r="W200" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X200" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T4-?</v>
+        <v>M2-T4-?</v>
       </c>
     </row>
     <row r="201" spans="1:24" x14ac:dyDescent="0.25">
@@ -17652,11 +17657,11 @@
       </c>
       <c r="W201" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X201" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T4-?</v>
+        <v>M2-T4-?</v>
       </c>
     </row>
     <row r="202" spans="1:24" x14ac:dyDescent="0.25">
@@ -19134,11 +19139,11 @@
       </c>
       <c r="W220" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X220" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-R1</v>
+        <v>M2-T7-R1</v>
       </c>
     </row>
     <row r="221" spans="1:24" x14ac:dyDescent="0.25">
@@ -19212,11 +19217,11 @@
       </c>
       <c r="W221" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X221" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-S1</v>
+        <v>M2-T7-S1</v>
       </c>
     </row>
     <row r="222" spans="1:24" x14ac:dyDescent="0.25">
@@ -19290,11 +19295,11 @@
       </c>
       <c r="W222" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X222" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-D1</v>
+        <v>M2-T7-D1</v>
       </c>
     </row>
     <row r="223" spans="1:24" x14ac:dyDescent="0.25">
@@ -19368,11 +19373,11 @@
       </c>
       <c r="W223" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X223" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-R4</v>
+        <v>M2-T7-R4</v>
       </c>
     </row>
     <row r="224" spans="1:24" x14ac:dyDescent="0.25">
@@ -19446,11 +19451,11 @@
       </c>
       <c r="W224" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X224" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-S4</v>
+        <v>M2-T7-S4</v>
       </c>
     </row>
     <row r="225" spans="1:24" x14ac:dyDescent="0.25">
@@ -19524,11 +19529,11 @@
       </c>
       <c r="W225" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X225" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T7-D4</v>
+        <v>M2-T7-D4</v>
       </c>
     </row>
     <row r="226" spans="1:24" x14ac:dyDescent="0.25">
@@ -21006,11 +21011,11 @@
       </c>
       <c r="W244" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X244" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-R1</v>
+        <v>M2-T14B-R1</v>
       </c>
     </row>
     <row r="245" spans="1:24" x14ac:dyDescent="0.25">
@@ -21084,11 +21089,11 @@
       </c>
       <c r="W245" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X245" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-S1</v>
+        <v>M2-T14B-S1</v>
       </c>
     </row>
     <row r="246" spans="1:24" x14ac:dyDescent="0.25">
@@ -21162,11 +21167,11 @@
       </c>
       <c r="W246" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X246" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-D1</v>
+        <v>M2-T14B-D1</v>
       </c>
     </row>
     <row r="247" spans="1:24" x14ac:dyDescent="0.25">
@@ -21240,11 +21245,11 @@
       </c>
       <c r="W247" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X247" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-R4</v>
+        <v>M2-T14B-R4</v>
       </c>
     </row>
     <row r="248" spans="1:24" x14ac:dyDescent="0.25">
@@ -21318,11 +21323,11 @@
       </c>
       <c r="W248" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X248" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-S4</v>
+        <v>M2-T14B-S4</v>
       </c>
     </row>
     <row r="249" spans="1:24" x14ac:dyDescent="0.25">
@@ -21396,11 +21401,11 @@
       </c>
       <c r="W249" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X249" s="3" t="str">
         <f t="shared" si="11"/>
-        <v>F2-T14B-D4</v>
+        <v>M2-T14B-D4</v>
       </c>
     </row>
     <row r="250" spans="1:24" x14ac:dyDescent="0.25">
@@ -22175,7 +22180,7 @@
         <v>R4</v>
       </c>
       <c r="W259" s="3" t="str">
-        <f t="shared" ref="W259:W322" si="13">IF(AND(B259=0,E259=1),"F1",IF(AND(B259=0,E259=2),"F2",IF(AND(B259=1,E259=1),"M1",IF(AND(B259=1,E259=2),"F2","?"))))</f>
+        <f t="shared" ref="W259:W322" si="13">IF(AND(B259=0,E259=1),"F1",IF(AND(B259=0,E259=2),"F2",IF(AND(B259=1,E259=1),"M1",IF(AND(B259=1,E259=2),"M2","?"))))</f>
         <v>F2</v>
       </c>
       <c r="X259" s="3" t="str">
@@ -22878,11 +22883,11 @@
       </c>
       <c r="W268" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X268" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--R1</v>
+        <v>M2--R1</v>
       </c>
     </row>
     <row r="269" spans="1:24" x14ac:dyDescent="0.25">
@@ -22956,11 +22961,11 @@
       </c>
       <c r="W269" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X269" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--S1</v>
+        <v>M2--S1</v>
       </c>
     </row>
     <row r="270" spans="1:24" x14ac:dyDescent="0.25">
@@ -23034,11 +23039,11 @@
       </c>
       <c r="W270" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X270" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--D1</v>
+        <v>M2--D1</v>
       </c>
     </row>
     <row r="271" spans="1:24" x14ac:dyDescent="0.25">
@@ -23112,11 +23117,11 @@
       </c>
       <c r="W271" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X271" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--R4</v>
+        <v>M2--R4</v>
       </c>
     </row>
     <row r="272" spans="1:24" x14ac:dyDescent="0.25">
@@ -23190,11 +23195,11 @@
       </c>
       <c r="W272" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X272" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--S4</v>
+        <v>M2--S4</v>
       </c>
     </row>
     <row r="273" spans="1:24" x14ac:dyDescent="0.25">
@@ -23268,11 +23273,11 @@
       </c>
       <c r="W273" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X273" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2--D4</v>
+        <v>M2--D4</v>
       </c>
     </row>
     <row r="274" spans="1:24" x14ac:dyDescent="0.25">
@@ -24750,11 +24755,11 @@
       </c>
       <c r="W292" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X292" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-R1</v>
+        <v>M2-T18-R1</v>
       </c>
     </row>
     <row r="293" spans="1:24" x14ac:dyDescent="0.25">
@@ -24828,11 +24833,11 @@
       </c>
       <c r="W293" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X293" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-S1</v>
+        <v>M2-T18-S1</v>
       </c>
     </row>
     <row r="294" spans="1:24" x14ac:dyDescent="0.25">
@@ -24906,11 +24911,11 @@
       </c>
       <c r="W294" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X294" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-D1</v>
+        <v>M2-T18-D1</v>
       </c>
     </row>
     <row r="295" spans="1:24" x14ac:dyDescent="0.25">
@@ -24984,11 +24989,11 @@
       </c>
       <c r="W295" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X295" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-R4</v>
+        <v>M2-T18-R4</v>
       </c>
     </row>
     <row r="296" spans="1:24" x14ac:dyDescent="0.25">
@@ -25062,11 +25067,11 @@
       </c>
       <c r="W296" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X296" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-S4</v>
+        <v>M2-T18-S4</v>
       </c>
     </row>
     <row r="297" spans="1:24" x14ac:dyDescent="0.25">
@@ -25140,11 +25145,11 @@
       </c>
       <c r="W297" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X297" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T18-D4</v>
+        <v>M2-T18-D4</v>
       </c>
     </row>
     <row r="298" spans="1:24" x14ac:dyDescent="0.25">
@@ -26622,11 +26627,11 @@
       </c>
       <c r="W316" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X316" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-R1</v>
+        <v>M2-T17-R1</v>
       </c>
     </row>
     <row r="317" spans="1:24" x14ac:dyDescent="0.25">
@@ -26700,11 +26705,11 @@
       </c>
       <c r="W317" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X317" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-S1</v>
+        <v>M2-T17-S1</v>
       </c>
     </row>
     <row r="318" spans="1:24" x14ac:dyDescent="0.25">
@@ -26778,11 +26783,11 @@
       </c>
       <c r="W318" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X318" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-D1</v>
+        <v>M2-T17-D1</v>
       </c>
     </row>
     <row r="319" spans="1:24" x14ac:dyDescent="0.25">
@@ -26856,11 +26861,11 @@
       </c>
       <c r="W319" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X319" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-R4</v>
+        <v>M2-T17-R4</v>
       </c>
     </row>
     <row r="320" spans="1:24" x14ac:dyDescent="0.25">
@@ -26934,11 +26939,11 @@
       </c>
       <c r="W320" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X320" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-S4</v>
+        <v>M2-T17-S4</v>
       </c>
     </row>
     <row r="321" spans="1:24" x14ac:dyDescent="0.25">
@@ -27012,11 +27017,11 @@
       </c>
       <c r="W321" s="3" t="str">
         <f t="shared" si="13"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X321" s="3" t="str">
         <f t="shared" si="14"/>
-        <v>F2-T17-D4</v>
+        <v>M2-T17-D4</v>
       </c>
     </row>
     <row r="322" spans="1:24" x14ac:dyDescent="0.25">
@@ -27167,7 +27172,7 @@
         <v>S1</v>
       </c>
       <c r="W323" s="3" t="str">
-        <f t="shared" ref="W323:W369" si="16">IF(AND(B323=0,E323=1),"F1",IF(AND(B323=0,E323=2),"F2",IF(AND(B323=1,E323=1),"M1",IF(AND(B323=1,E323=2),"F2","?"))))</f>
+        <f t="shared" ref="W323:W369" si="16">IF(AND(B323=0,E323=1),"F1",IF(AND(B323=0,E323=2),"F2",IF(AND(B323=1,E323=1),"M1",IF(AND(B323=1,E323=2),"M2","?"))))</f>
         <v>F1</v>
       </c>
       <c r="X323" s="3" t="str">
@@ -28494,11 +28499,11 @@
       </c>
       <c r="W340" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X340" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-R1</v>
+        <v>M2-T19-R1</v>
       </c>
     </row>
     <row r="341" spans="1:24" x14ac:dyDescent="0.25">
@@ -28572,11 +28577,11 @@
       </c>
       <c r="W341" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X341" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-S1</v>
+        <v>M2-T19-S1</v>
       </c>
     </row>
     <row r="342" spans="1:24" x14ac:dyDescent="0.25">
@@ -28650,11 +28655,11 @@
       </c>
       <c r="W342" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X342" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-D1</v>
+        <v>M2-T19-D1</v>
       </c>
     </row>
     <row r="343" spans="1:24" x14ac:dyDescent="0.25">
@@ -28728,11 +28733,11 @@
       </c>
       <c r="W343" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X343" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-R4</v>
+        <v>M2-T19-R4</v>
       </c>
     </row>
     <row r="344" spans="1:24" x14ac:dyDescent="0.25">
@@ -28806,11 +28811,11 @@
       </c>
       <c r="W344" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X344" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-S4</v>
+        <v>M2-T19-S4</v>
       </c>
     </row>
     <row r="345" spans="1:24" x14ac:dyDescent="0.25">
@@ -28884,11 +28889,11 @@
       </c>
       <c r="W345" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X345" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2-T19-D4</v>
+        <v>M2-T19-D4</v>
       </c>
     </row>
     <row r="346" spans="1:24" x14ac:dyDescent="0.25">
@@ -30366,11 +30371,11 @@
       </c>
       <c r="W364" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X364" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--R1</v>
+        <v>M2--R1</v>
       </c>
     </row>
     <row r="365" spans="1:24" x14ac:dyDescent="0.25">
@@ -30444,11 +30449,11 @@
       </c>
       <c r="W365" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X365" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--S1</v>
+        <v>M2--S1</v>
       </c>
     </row>
     <row r="366" spans="1:24" x14ac:dyDescent="0.25">
@@ -30522,11 +30527,11 @@
       </c>
       <c r="W366" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X366" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--D1</v>
+        <v>M2--D1</v>
       </c>
     </row>
     <row r="367" spans="1:24" x14ac:dyDescent="0.25">
@@ -30600,11 +30605,11 @@
       </c>
       <c r="W367" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X367" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--R4</v>
+        <v>M2--R4</v>
       </c>
     </row>
     <row r="368" spans="1:24" x14ac:dyDescent="0.25">
@@ -30678,11 +30683,11 @@
       </c>
       <c r="W368" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X368" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--S4</v>
+        <v>M2--S4</v>
       </c>
     </row>
     <row r="369" spans="1:24" x14ac:dyDescent="0.25">
@@ -30756,11 +30761,11 @@
       </c>
       <c r="W369" s="3" t="str">
         <f t="shared" si="16"/>
-        <v>F2</v>
+        <v>M2</v>
       </c>
       <c r="X369" s="3" t="str">
         <f t="shared" si="17"/>
-        <v>F2--D4</v>
+        <v>M2--D4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix error with 13 trials
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -1849,7 +1849,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,9 +2743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y391" sqref="Y391"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P361" sqref="P361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32361,7 +32361,7 @@
         <v>0</v>
       </c>
       <c r="P338" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q338" s="3" t="s">
         <v>242</v>
@@ -32445,7 +32445,7 @@
         <v>0</v>
       </c>
       <c r="P339" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q339" s="3" t="s">
         <v>242</v>
@@ -32529,7 +32529,7 @@
         <v>0</v>
       </c>
       <c r="P340" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q340" s="3" t="s">
         <v>242</v>
@@ -32613,7 +32613,7 @@
         <v>0</v>
       </c>
       <c r="P341" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q341" s="3" t="s">
         <v>242</v>
@@ -32697,7 +32697,7 @@
         <v>0</v>
       </c>
       <c r="P342" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q342" s="3" t="s">
         <v>242</v>
@@ -32781,7 +32781,7 @@
         <v>0</v>
       </c>
       <c r="P343" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q343" s="3" t="s">
         <v>242</v>
@@ -32865,7 +32865,7 @@
         <v>0</v>
       </c>
       <c r="P344" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q344" s="3" t="s">
         <v>242</v>
@@ -32949,7 +32949,7 @@
         <v>0</v>
       </c>
       <c r="P345" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q345" s="3" t="s">
         <v>242</v>
@@ -33033,7 +33033,7 @@
         <v>0</v>
       </c>
       <c r="P346" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q346" s="3" t="s">
         <v>242</v>
@@ -33117,7 +33117,7 @@
         <v>0</v>
       </c>
       <c r="P347" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q347" s="3" t="s">
         <v>242</v>
@@ -33201,7 +33201,7 @@
         <v>0</v>
       </c>
       <c r="P348" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q348" s="3" t="s">
         <v>242</v>
@@ -33285,7 +33285,7 @@
         <v>0</v>
       </c>
       <c r="P349" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q349" s="3" t="s">
         <v>242</v>
@@ -33369,7 +33369,7 @@
         <v>0</v>
       </c>
       <c r="P350" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q350" s="3" t="s">
         <v>242</v>
@@ -33453,7 +33453,7 @@
         <v>0</v>
       </c>
       <c r="P351" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q351" s="3" t="s">
         <v>242</v>
@@ -33537,7 +33537,7 @@
         <v>0</v>
       </c>
       <c r="P352" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q352" s="3" t="s">
         <v>242</v>
@@ -33621,7 +33621,7 @@
         <v>0</v>
       </c>
       <c r="P353" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q353" s="3" t="s">
         <v>242</v>
@@ -33705,7 +33705,7 @@
         <v>0</v>
       </c>
       <c r="P354" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q354" s="3" t="s">
         <v>242</v>
@@ -33789,7 +33789,7 @@
         <v>0</v>
       </c>
       <c r="P355" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q355" s="3" t="s">
         <v>242</v>
@@ -33873,7 +33873,7 @@
         <v>0</v>
       </c>
       <c r="P356" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q356" s="3" t="s">
         <v>242</v>
@@ -33957,7 +33957,7 @@
         <v>0</v>
       </c>
       <c r="P357" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q357" s="3" t="s">
         <v>242</v>
@@ -34041,7 +34041,7 @@
         <v>0</v>
       </c>
       <c r="P358" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q358" s="3" t="s">
         <v>242</v>
@@ -34125,7 +34125,7 @@
         <v>0</v>
       </c>
       <c r="P359" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q359" s="3" t="s">
         <v>242</v>
@@ -34209,7 +34209,7 @@
         <v>0</v>
       </c>
       <c r="P360" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q360" s="3" t="s">
         <v>242</v>
@@ -34293,7 +34293,7 @@
         <v>0</v>
       </c>
       <c r="P361" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q361" s="3" t="s">
         <v>242</v>
@@ -36352,7 +36352,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37104,8 +37104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add tune or corecases to list
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\iwccla\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AEP" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">base!$A$1:$AB$393</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tune!$A$1:$AA$23</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="475">
   <si>
     <t>Trial</t>
   </si>
@@ -1478,15 +1483,6 @@
   </si>
   <si>
     <t>Now in the trial list but not ran</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1870,7 +1866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2747,9 +2743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB393"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37026,9 +37022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37037,23 +37033,22 @@
     <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="3"/>
-    <col min="12" max="12" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="3"/>
-    <col min="15" max="15" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" style="3" customWidth="1"/>
     <col min="19" max="19" width="7.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="8.5703125" style="3" customWidth="1"/>
+    <col min="20" max="22" width="8.5703125" style="3" customWidth="1"/>
     <col min="23" max="23" width="5.28515625" style="3" customWidth="1"/>
     <col min="24" max="24" width="6.7109375" style="3" customWidth="1"/>
     <col min="25" max="25" width="4.5703125" style="3" customWidth="1"/>
@@ -37211,17 +37206,21 @@
       <c r="V2" s="3">
         <v>0.2</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>264</v>
+      <c r="W2" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X2" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D2,info!$C$11:$D$19), F2*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y2" s="3" t="str">
+        <f t="shared" ref="Y2:Y25" si="0">IF(AND(B2=0,E2=1),"F1",IF(AND(B2=0,E2=2),"F2",IF(AND(B2=1,E2=1),"M1",IF(AND(B2=1,E2=2),"M2","?"))))</f>
+        <v>F1</v>
+      </c>
+      <c r="Z2" s="3" t="str">
+        <f t="shared" ref="Z2:Z25" si="1">CONCATENATE($Y2,"-",$W2,"-",$X2)</f>
+        <v>F1-T2-R1</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>437</v>
@@ -37294,17 +37293,21 @@
       <c r="V3" s="3">
         <v>0.2</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>266</v>
+      <c r="W3" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X3" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D3,info!$C$11:$D$19), F3*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>F1</v>
+      </c>
+      <c r="Z3" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-T2-D1</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>437</v>
@@ -37377,17 +37380,21 @@
       <c r="V4" s="3">
         <v>0.2</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>264</v>
+      <c r="W4" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X4" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D4,info!$C$11:$D$19), F4*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>F2</v>
+      </c>
+      <c r="Z4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-T2-R1</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>437</v>
@@ -37460,17 +37467,21 @@
       <c r="V5" s="3">
         <v>0.2</v>
       </c>
-      <c r="W5" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>266</v>
+      <c r="W5" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X5" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D5,info!$C$11:$D$19), F5*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>F2</v>
+      </c>
+      <c r="Z5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-T2-D1</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>437</v>
@@ -37543,19 +37554,20 @@
       <c r="V6" s="3">
         <v>0.2</v>
       </c>
-      <c r="W6" s="3" t="s">
-        <v>244</v>
+      <c r="W6" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X6" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D6,info!$C$11:$D$19), F6*100)</f>
         <v>R1</v>
       </c>
       <c r="Y6" s="3" t="str">
-        <f>IF(AND(B6=0,E6=1),"F1",IF(AND(B6=0,E6=2),"F2",IF(AND(B6=1,E6=1),"M1",IF(AND(B6=1,E6=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z6" s="3" t="str">
-        <f>CONCATENATE($Y6,"-",$W6,"-",$X6)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-R1</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -37629,19 +37641,20 @@
       <c r="V7" s="3">
         <v>0.2</v>
       </c>
-      <c r="W7" s="3" t="s">
-        <v>244</v>
+      <c r="W7" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X7" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D7,info!$C$11:$D$19), F7*100)</f>
         <v>S1</v>
       </c>
       <c r="Y7" s="3" t="str">
-        <f>IF(AND(B7=0,E7=1),"F1",IF(AND(B7=0,E7=2),"F2",IF(AND(B7=1,E7=1),"M1",IF(AND(B7=1,E7=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z7" s="3" t="str">
-        <f>CONCATENATE($Y7,"-",$W7,"-",$X7)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-S1</v>
       </c>
       <c r="AA7" s="3" t="s">
@@ -37715,19 +37728,20 @@
       <c r="V8" s="3">
         <v>0.2</v>
       </c>
-      <c r="W8" s="3" t="s">
-        <v>244</v>
+      <c r="W8" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X8" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D8,info!$C$11:$D$19), F8*100)</f>
         <v>D1</v>
       </c>
       <c r="Y8" s="3" t="str">
-        <f>IF(AND(B8=0,E8=1),"F1",IF(AND(B8=0,E8=2),"F2",IF(AND(B8=1,E8=1),"M1",IF(AND(B8=1,E8=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z8" s="3" t="str">
-        <f>CONCATENATE($Y8,"-",$W8,"-",$X8)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-D1</v>
       </c>
       <c r="AA8" s="3" t="s">
@@ -37801,19 +37815,20 @@
       <c r="V9" s="3">
         <v>0.2</v>
       </c>
-      <c r="W9" s="3" t="s">
-        <v>244</v>
+      <c r="W9" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X9" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D9,info!$C$11:$D$19), F9*100)</f>
         <v>R1</v>
       </c>
       <c r="Y9" s="3" t="str">
-        <f>IF(AND(B9=0,E9=1),"F1",IF(AND(B9=0,E9=2),"F2",IF(AND(B9=1,E9=1),"M1",IF(AND(B9=1,E9=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z9" s="3" t="str">
-        <f>CONCATENATE($Y9,"-",$W9,"-",$X9)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-R1</v>
       </c>
       <c r="AA9" s="3" t="s">
@@ -37887,19 +37902,20 @@
       <c r="V10" s="3">
         <v>0.2</v>
       </c>
-      <c r="W10" s="3" t="s">
-        <v>244</v>
+      <c r="W10" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X10" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D10,info!$C$11:$D$19), F10*100)</f>
         <v>S1</v>
       </c>
       <c r="Y10" s="3" t="str">
-        <f>IF(AND(B10=0,E10=1),"F1",IF(AND(B10=0,E10=2),"F2",IF(AND(B10=1,E10=1),"M1",IF(AND(B10=1,E10=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z10" s="3" t="str">
-        <f>CONCATENATE($Y10,"-",$W10,"-",$X10)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-S1</v>
       </c>
       <c r="AA10" s="3" t="s">
@@ -37973,19 +37989,20 @@
       <c r="V11" s="3">
         <v>0.2</v>
       </c>
-      <c r="W11" s="3" t="s">
-        <v>244</v>
+      <c r="W11" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X11" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D11,info!$C$11:$D$19), F11*100)</f>
         <v>D1</v>
       </c>
       <c r="Y11" s="3" t="str">
-        <f>IF(AND(B11=0,E11=1),"F1",IF(AND(B11=0,E11=2),"F2",IF(AND(B11=1,E11=1),"M1",IF(AND(B11=1,E11=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z11" s="3" t="str">
-        <f>CONCATENATE($Y11,"-",$W11,"-",$X11)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-D1</v>
       </c>
       <c r="AA11" s="3" t="s">
@@ -38059,20 +38076,21 @@
       <c r="V12" s="3">
         <v>0.2</v>
       </c>
-      <c r="W12" s="3" t="s">
-        <v>244</v>
+      <c r="W12" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X12" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D12,info!$C$11:$D$19), F12*100)</f>
         <v>R1</v>
       </c>
       <c r="Y12" s="3" t="str">
-        <f>IF(AND(B12=0,E12=1),"F1",IF(AND(B12=0,E12=2),"F2",IF(AND(B12=1,E12=1),"M1",IF(AND(B12=1,E12=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z12" s="3" t="str">
-        <f>CONCATENATE($Y12,"-",$W12,"-",$X12)</f>
-        <v>F1-T1-R1</v>
+        <f t="shared" si="1"/>
+        <v>F1-T3-R1</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>437</v>
@@ -38145,20 +38163,21 @@
       <c r="V13" s="3">
         <v>0.2</v>
       </c>
-      <c r="W13" s="3" t="s">
-        <v>244</v>
+      <c r="W13" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X13" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D13,info!$C$11:$D$19), F13*100)</f>
         <v>S1</v>
       </c>
       <c r="Y13" s="3" t="str">
-        <f>IF(AND(B13=0,E13=1),"F1",IF(AND(B13=0,E13=2),"F2",IF(AND(B13=1,E13=1),"M1",IF(AND(B13=1,E13=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z13" s="3" t="str">
-        <f>CONCATENATE($Y13,"-",$W13,"-",$X13)</f>
-        <v>F1-T1-S1</v>
+        <f t="shared" si="1"/>
+        <v>F1-T3-S1</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>437</v>
@@ -38231,20 +38250,21 @@
       <c r="V14" s="3">
         <v>0.2</v>
       </c>
-      <c r="W14" s="3" t="s">
-        <v>244</v>
+      <c r="W14" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X14" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D14,info!$C$11:$D$19), F14*100)</f>
         <v>D1</v>
       </c>
       <c r="Y14" s="3" t="str">
-        <f>IF(AND(B14=0,E14=1),"F1",IF(AND(B14=0,E14=2),"F2",IF(AND(B14=1,E14=1),"M1",IF(AND(B14=1,E14=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z14" s="3" t="str">
-        <f>CONCATENATE($Y14,"-",$W14,"-",$X14)</f>
-        <v>F1-T1-D1</v>
+        <f t="shared" si="1"/>
+        <v>F1-T3-D1</v>
       </c>
       <c r="AA14" s="3" t="s">
         <v>437</v>
@@ -38317,20 +38337,21 @@
       <c r="V15" s="3">
         <v>0.2</v>
       </c>
-      <c r="W15" s="3" t="s">
-        <v>244</v>
+      <c r="W15" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X15" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D15,info!$C$11:$D$19), F15*100)</f>
         <v>R1</v>
       </c>
       <c r="Y15" s="3" t="str">
-        <f>IF(AND(B15=0,E15=1),"F1",IF(AND(B15=0,E15=2),"F2",IF(AND(B15=1,E15=1),"M1",IF(AND(B15=1,E15=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z15" s="3" t="str">
-        <f>CONCATENATE($Y15,"-",$W15,"-",$X15)</f>
-        <v>F2-T1-R1</v>
+        <f t="shared" si="1"/>
+        <v>F2-T3-R1</v>
       </c>
       <c r="AA15" s="3" t="s">
         <v>437</v>
@@ -38403,20 +38424,21 @@
       <c r="V16" s="3">
         <v>0.2</v>
       </c>
-      <c r="W16" s="3" t="s">
-        <v>244</v>
+      <c r="W16" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X16" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D16,info!$C$11:$D$19), F16*100)</f>
         <v>S1</v>
       </c>
       <c r="Y16" s="3" t="str">
-        <f>IF(AND(B16=0,E16=1),"F1",IF(AND(B16=0,E16=2),"F2",IF(AND(B16=1,E16=1),"M1",IF(AND(B16=1,E16=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z16" s="3" t="str">
-        <f>CONCATENATE($Y16,"-",$W16,"-",$X16)</f>
-        <v>F2-T1-S1</v>
+        <f t="shared" si="1"/>
+        <v>F2-T3-S1</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>437</v>
@@ -38489,20 +38511,21 @@
       <c r="V17" s="3">
         <v>0.2</v>
       </c>
-      <c r="W17" s="3" t="s">
-        <v>244</v>
+      <c r="W17" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
       </c>
       <c r="X17" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D17,info!$C$11:$D$19), F17*100)</f>
         <v>D1</v>
       </c>
       <c r="Y17" s="3" t="str">
-        <f>IF(AND(B17=0,E17=1),"F1",IF(AND(B17=0,E17=2),"F2",IF(AND(B17=1,E17=1),"M1",IF(AND(B17=1,E17=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z17" s="3" t="str">
-        <f>CONCATENATE($Y17,"-",$W17,"-",$X17)</f>
-        <v>F2-T1-D1</v>
+        <f t="shared" si="1"/>
+        <v>F2-T3-D1</v>
       </c>
       <c r="AA17" s="3" t="s">
         <v>437</v>
@@ -38575,19 +38598,20 @@
       <c r="V18" s="3">
         <v>0.2</v>
       </c>
-      <c r="W18" s="3" t="s">
-        <v>244</v>
+      <c r="W18" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X18" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D18,info!$C$11:$D$19), F18*100)</f>
         <v>R4</v>
       </c>
       <c r="Y18" s="3" t="str">
-        <f>IF(AND(B18=0,E18=1),"F1",IF(AND(B18=0,E18=2),"F2",IF(AND(B18=1,E18=1),"M1",IF(AND(B18=1,E18=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z18" s="3" t="str">
-        <f>CONCATENATE($Y18,"-",$W18,"-",$X18)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-R4</v>
       </c>
       <c r="AA18" s="3" t="s">
@@ -38661,19 +38685,20 @@
       <c r="V19" s="3">
         <v>0.2</v>
       </c>
-      <c r="W19" s="3" t="s">
-        <v>244</v>
+      <c r="W19" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X19" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D19,info!$C$11:$D$19), F19*100)</f>
         <v>D4</v>
       </c>
       <c r="Y19" s="3" t="str">
-        <f>IF(AND(B19=0,E19=1),"F1",IF(AND(B19=0,E19=2),"F2",IF(AND(B19=1,E19=1),"M1",IF(AND(B19=1,E19=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z19" s="3" t="str">
-        <f>CONCATENATE($Y19,"-",$W19,"-",$X19)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-D4</v>
       </c>
       <c r="AA19" s="3" t="s">
@@ -38747,19 +38772,20 @@
       <c r="V20" s="3">
         <v>0.2</v>
       </c>
-      <c r="W20" s="3" t="s">
-        <v>244</v>
+      <c r="W20" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X20" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D20,info!$C$11:$D$19), F20*100)</f>
         <v>R4</v>
       </c>
       <c r="Y20" s="3" t="str">
-        <f>IF(AND(B20=0,E20=1),"F1",IF(AND(B20=0,E20=2),"F2",IF(AND(B20=1,E20=1),"M1",IF(AND(B20=1,E20=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z20" s="3" t="str">
-        <f>CONCATENATE($Y20,"-",$W20,"-",$X20)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-R4</v>
       </c>
       <c r="AA20" s="3" t="s">
@@ -38833,19 +38859,20 @@
       <c r="V21" s="3">
         <v>0.2</v>
       </c>
-      <c r="W21" s="3" t="s">
-        <v>244</v>
+      <c r="W21" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X21" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D21,info!$C$11:$D$19), F21*100)</f>
         <v>D4</v>
       </c>
       <c r="Y21" s="3" t="str">
-        <f>IF(AND(B21=0,E21=1),"F1",IF(AND(B21=0,E21=2),"F2",IF(AND(B21=1,E21=1),"M1",IF(AND(B21=1,E21=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z21" s="3" t="str">
-        <f>CONCATENATE($Y21,"-",$W21,"-",$X21)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-D4</v>
       </c>
       <c r="AA21" s="3" t="s">
@@ -38919,19 +38946,20 @@
       <c r="V22" s="3">
         <v>0.2</v>
       </c>
-      <c r="W22" s="3" t="s">
-        <v>244</v>
+      <c r="W22" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X22" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D22,info!$C$11:$D$19), F22*100)</f>
         <v>R7</v>
       </c>
       <c r="Y22" s="3" t="str">
-        <f>IF(AND(B22=0,E22=1),"F1",IF(AND(B22=0,E22=2),"F2",IF(AND(B22=1,E22=1),"M1",IF(AND(B22=1,E22=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z22" s="3" t="str">
-        <f>CONCATENATE($Y22,"-",$W22,"-",$X22)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-R7</v>
       </c>
       <c r="AA22" s="3" t="s">
@@ -39005,19 +39033,20 @@
       <c r="V23" s="3">
         <v>0.2</v>
       </c>
-      <c r="W23" s="3" t="s">
-        <v>244</v>
+      <c r="W23" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X23" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D23,info!$C$11:$D$19), F23*100)</f>
         <v>D7</v>
       </c>
       <c r="Y23" s="3" t="str">
-        <f>IF(AND(B23=0,E23=1),"F1",IF(AND(B23=0,E23=2),"F2",IF(AND(B23=1,E23=1),"M1",IF(AND(B23=1,E23=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F1</v>
       </c>
       <c r="Z23" s="3" t="str">
-        <f>CONCATENATE($Y23,"-",$W23,"-",$X23)</f>
+        <f t="shared" si="1"/>
         <v>F1-T1-D7</v>
       </c>
       <c r="AA23" s="3" t="s">
@@ -39091,19 +39120,20 @@
       <c r="V24" s="3">
         <v>0.2</v>
       </c>
-      <c r="W24" s="3" t="s">
-        <v>244</v>
+      <c r="W24" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X24" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D24,info!$C$11:$D$19), F24*100)</f>
         <v>R7</v>
       </c>
       <c r="Y24" s="3" t="str">
-        <f>IF(AND(B24=0,E24=1),"F1",IF(AND(B24=0,E24=2),"F2",IF(AND(B24=1,E24=1),"M1",IF(AND(B24=1,E24=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z24" s="3" t="str">
-        <f>CONCATENATE($Y24,"-",$W24,"-",$X24)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-R7</v>
       </c>
       <c r="AA24" s="3" t="s">
@@ -39177,19 +39207,20 @@
       <c r="V25" s="3">
         <v>0.2</v>
       </c>
-      <c r="W25" s="3" t="s">
-        <v>244</v>
+      <c r="W25" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
       </c>
       <c r="X25" s="3" t="str">
         <f>CONCATENATE(LOOKUP(D25,info!$C$11:$D$19), F25*100)</f>
         <v>D7</v>
       </c>
       <c r="Y25" s="3" t="str">
-        <f>IF(AND(B25=0,E25=1),"F1",IF(AND(B25=0,E25=2),"F2",IF(AND(B25=1,E25=1),"M1",IF(AND(B25=1,E25=2),"M2","?"))))</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="Z25" s="3" t="str">
-        <f>CONCATENATE($Y25,"-",$W25,"-",$X25)</f>
+        <f t="shared" si="1"/>
         <v>F2-T1-D7</v>
       </c>
       <c r="AA25" s="3" t="s">

</xml_diff>

<commit_message>
Add natural mortality trials to tune
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AEP" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="475">
   <si>
     <t>Trial</t>
   </si>
@@ -2743,9 +2743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB393"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K391" sqref="K391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37020,11 +37020,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37219,11 +37219,8 @@
         <v>F1</v>
       </c>
       <c r="Z2" s="3" t="str">
-        <f t="shared" ref="Z2:Z25" si="1">CONCATENATE($Y2,"-",$W2,"-",$X2)</f>
+        <f t="shared" ref="Z2:Z49" si="1">CONCATENATE($Y2,"-",$W2,"-",$X2)</f>
         <v>F1-T2-R1</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -37309,9 +37306,6 @@
         <f t="shared" si="1"/>
         <v>F1-T2-D1</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -37396,9 +37390,6 @@
         <f t="shared" si="1"/>
         <v>F2-T2-R1</v>
       </c>
-      <c r="AA4" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -37483,9 +37474,6 @@
         <f t="shared" si="1"/>
         <v>F2-T2-D1</v>
       </c>
-      <c r="AA5" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -37570,9 +37558,6 @@
         <f t="shared" si="1"/>
         <v>F1-T1-R1</v>
       </c>
-      <c r="AA6" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -37657,9 +37642,6 @@
         <f t="shared" si="1"/>
         <v>F1-T1-S1</v>
       </c>
-      <c r="AA7" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -37744,9 +37726,6 @@
         <f t="shared" si="1"/>
         <v>F1-T1-D1</v>
       </c>
-      <c r="AA8" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -37831,9 +37810,6 @@
         <f t="shared" si="1"/>
         <v>F2-T1-R1</v>
       </c>
-      <c r="AA9" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -37918,9 +37894,6 @@
         <f t="shared" si="1"/>
         <v>F2-T1-S1</v>
       </c>
-      <c r="AA10" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -38005,9 +37978,6 @@
         <f t="shared" si="1"/>
         <v>F2-T1-D1</v>
       </c>
-      <c r="AA11" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -38092,9 +38062,6 @@
         <f t="shared" si="1"/>
         <v>F1-T3-R1</v>
       </c>
-      <c r="AA12" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -38179,9 +38146,6 @@
         <f t="shared" si="1"/>
         <v>F1-T3-S1</v>
       </c>
-      <c r="AA13" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -38266,9 +38230,6 @@
         <f t="shared" si="1"/>
         <v>F1-T3-D1</v>
       </c>
-      <c r="AA14" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -38353,9 +38314,6 @@
         <f t="shared" si="1"/>
         <v>F2-T3-R1</v>
       </c>
-      <c r="AA15" s="3" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -38440,11 +38398,8 @@
         <f t="shared" si="1"/>
         <v>F2-T3-S1</v>
       </c>
-      <c r="AA16" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>300</v>
       </c>
@@ -38527,11 +38482,8 @@
         <f t="shared" si="1"/>
         <v>F2-T3-D1</v>
       </c>
-      <c r="AA17" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>300</v>
       </c>
@@ -38614,11 +38566,8 @@
         <f t="shared" si="1"/>
         <v>F1-T1-R4</v>
       </c>
-      <c r="AA18" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>300</v>
       </c>
@@ -38701,11 +38650,8 @@
         <f t="shared" si="1"/>
         <v>F1-T1-D4</v>
       </c>
-      <c r="AA19" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>300</v>
       </c>
@@ -38788,11 +38734,8 @@
         <f t="shared" si="1"/>
         <v>F2-T1-R4</v>
       </c>
-      <c r="AA20" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>300</v>
       </c>
@@ -38875,11 +38818,8 @@
         <f t="shared" si="1"/>
         <v>F2-T1-D4</v>
       </c>
-      <c r="AA21" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>300</v>
       </c>
@@ -38962,11 +38902,8 @@
         <f t="shared" si="1"/>
         <v>F1-T1-R7</v>
       </c>
-      <c r="AA22" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>300</v>
       </c>
@@ -39049,11 +38986,8 @@
         <f t="shared" si="1"/>
         <v>F1-T1-D7</v>
       </c>
-      <c r="AA23" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>300</v>
       </c>
@@ -39136,11 +39070,8 @@
         <f t="shared" si="1"/>
         <v>F2-T1-R7</v>
       </c>
-      <c r="AA24" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>300</v>
       </c>
@@ -39223,8 +39154,2021 @@
         <f t="shared" si="1"/>
         <v>F2-T1-D7</v>
       </c>
-      <c r="AA25" s="3" t="s">
-        <v>437</v>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>300</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <v>400</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H26" s="3">
+        <v>5</v>
+      </c>
+      <c r="I26" s="4">
+        <v>7</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>30</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R26" s="3">
+        <v>0</v>
+      </c>
+      <c r="S26" s="3">
+        <v>0</v>
+      </c>
+      <c r="T26" s="3">
+        <v>0</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V26" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W26" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X26" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D26,info!$C$11:$D$19), F26*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y26" s="3" t="str">
+        <f t="shared" ref="Y26:Y49" si="2">IF(AND(B26=0,E26=1),"F1",IF(AND(B26=0,E26=2),"F2",IF(AND(B26=1,E26=1),"M1",IF(AND(B26=1,E26=2),"M2","?"))))</f>
+        <v>M1</v>
+      </c>
+      <c r="Z26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T2-R1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>300</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>400</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>7</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <v>30</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
+        <v>0</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V27" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W27" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X27" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D27,info!$C$11:$D$19), F27*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y27" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T2-D1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>300</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>400</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>7</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>30</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W28" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X28" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D28,info!$C$11:$D$19), F28*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y28" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T2-R1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>300</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>400</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H29" s="3">
+        <v>5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>7</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>30</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W29" s="3" t="str">
+        <f>AEP!$A$17</f>
+        <v>T2</v>
+      </c>
+      <c r="X29" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D29,info!$C$11:$D$19), F29*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y29" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T2-D1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>300</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <v>400</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H30" s="3">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4">
+        <v>7</v>
+      </c>
+      <c r="J30" s="4">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>30</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+      <c r="S30" s="3">
+        <v>0</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V30" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W30" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X30" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D30,info!$C$11:$D$19), F30*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-R1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>300</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>400</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5</v>
+      </c>
+      <c r="I31" s="4">
+        <v>7</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>30</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V31" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W31" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X31" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D31,info!$C$11:$D$19), F31*100)</f>
+        <v>S1</v>
+      </c>
+      <c r="Y31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-S1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>300</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3">
+        <v>400</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H32" s="3">
+        <v>5</v>
+      </c>
+      <c r="I32" s="4">
+        <v>7</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0</v>
+      </c>
+      <c r="L32" s="3">
+        <v>30</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="3">
+        <v>0</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V32" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W32" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X32" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D32,info!$C$11:$D$19), F32*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-D1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>300</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>400</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5</v>
+      </c>
+      <c r="I33" s="4">
+        <v>7</v>
+      </c>
+      <c r="J33" s="4">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0</v>
+      </c>
+      <c r="L33" s="3">
+        <v>30</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+      <c r="S33" s="3">
+        <v>0</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0</v>
+      </c>
+      <c r="U33" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V33" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W33" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X33" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D33,info!$C$11:$D$19), F33*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-R1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>300</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3">
+        <v>400</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>5</v>
+      </c>
+      <c r="I34" s="4">
+        <v>7</v>
+      </c>
+      <c r="J34" s="4">
+        <v>1</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0</v>
+      </c>
+      <c r="L34" s="3">
+        <v>30</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0</v>
+      </c>
+      <c r="P34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="3">
+        <v>0</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V34" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W34" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X34" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D34,info!$C$11:$D$19), F34*100)</f>
+        <v>S1</v>
+      </c>
+      <c r="Y34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-S1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>300</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <v>400</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E35" s="3">
+        <v>2</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>5</v>
+      </c>
+      <c r="I35" s="4">
+        <v>7</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <v>30</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0</v>
+      </c>
+      <c r="P35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+      <c r="S35" s="3">
+        <v>0</v>
+      </c>
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W35" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X35" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D35,info!$C$11:$D$19), F35*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-D1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>300</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3">
+        <v>400</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5</v>
+      </c>
+      <c r="I36" s="4">
+        <v>7</v>
+      </c>
+      <c r="J36" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3">
+        <v>30</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+      <c r="S36" s="3">
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V36" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W36" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X36" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D36,info!$C$11:$D$19), F36*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z36" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T3-R1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>300</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>400</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>5</v>
+      </c>
+      <c r="I37" s="4">
+        <v>7</v>
+      </c>
+      <c r="J37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3">
+        <v>30</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0</v>
+      </c>
+      <c r="T37" s="3">
+        <v>0</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V37" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W37" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X37" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D37,info!$C$11:$D$19), F37*100)</f>
+        <v>S1</v>
+      </c>
+      <c r="Y37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T3-S1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>300</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3">
+        <v>400</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="4">
+        <v>7</v>
+      </c>
+      <c r="J38" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>30</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0</v>
+      </c>
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="3">
+        <v>0</v>
+      </c>
+      <c r="U38" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V38" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W38" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X38" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D38,info!$C$11:$D$19), F38*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y38" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z38" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T3-D1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>300</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3">
+        <v>400</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
+      </c>
+      <c r="I39" s="4">
+        <v>7</v>
+      </c>
+      <c r="J39" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3">
+        <v>30</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R39" s="3">
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
+        <v>0</v>
+      </c>
+      <c r="U39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W39" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X39" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D39,info!$C$11:$D$19), F39*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y39" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T3-R1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>300</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3">
+        <v>400</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H40" s="3">
+        <v>5</v>
+      </c>
+      <c r="I40" s="4">
+        <v>7</v>
+      </c>
+      <c r="J40" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <v>30</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R40" s="3">
+        <v>0</v>
+      </c>
+      <c r="S40" s="3">
+        <v>0</v>
+      </c>
+      <c r="T40" s="3">
+        <v>0</v>
+      </c>
+      <c r="U40" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V40" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W40" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X40" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D40,info!$C$11:$D$19), F40*100)</f>
+        <v>S1</v>
+      </c>
+      <c r="Y40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z40" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T3-S1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>300</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <v>400</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H41" s="3">
+        <v>5</v>
+      </c>
+      <c r="I41" s="4">
+        <v>7</v>
+      </c>
+      <c r="J41" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3">
+        <v>30</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0</v>
+      </c>
+      <c r="P41" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R41" s="3">
+        <v>0</v>
+      </c>
+      <c r="S41" s="3">
+        <v>0</v>
+      </c>
+      <c r="T41" s="3">
+        <v>0</v>
+      </c>
+      <c r="U41" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V41" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W41" s="3" t="str">
+        <f>AEP!$A$18</f>
+        <v>T3</v>
+      </c>
+      <c r="X41" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D41,info!$C$11:$D$19), F41*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y41" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T3-D1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>300</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3">
+        <v>400</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H42" s="3">
+        <v>5</v>
+      </c>
+      <c r="I42" s="4">
+        <v>7</v>
+      </c>
+      <c r="J42" s="4">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>30</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R42" s="3">
+        <v>0</v>
+      </c>
+      <c r="S42" s="3">
+        <v>0</v>
+      </c>
+      <c r="T42" s="3">
+        <v>0</v>
+      </c>
+      <c r="U42" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V42" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W42" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X42" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D42,info!$C$11:$D$19), F42*100)</f>
+        <v>R4</v>
+      </c>
+      <c r="Y42" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-R4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>300</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3">
+        <v>400</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H43" s="3">
+        <v>5</v>
+      </c>
+      <c r="I43" s="4">
+        <v>7</v>
+      </c>
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
+        <v>30</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0</v>
+      </c>
+      <c r="P43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R43" s="3">
+        <v>0</v>
+      </c>
+      <c r="S43" s="3">
+        <v>0</v>
+      </c>
+      <c r="T43" s="3">
+        <v>0</v>
+      </c>
+      <c r="U43" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V43" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W43" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X43" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D43,info!$C$11:$D$19), F43*100)</f>
+        <v>D4</v>
+      </c>
+      <c r="Y43" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z43" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-D4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>300</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3">
+        <v>400</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H44" s="3">
+        <v>5</v>
+      </c>
+      <c r="I44" s="4">
+        <v>7</v>
+      </c>
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>30</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O44" s="3">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R44" s="3">
+        <v>0</v>
+      </c>
+      <c r="S44" s="3">
+        <v>0</v>
+      </c>
+      <c r="T44" s="3">
+        <v>0</v>
+      </c>
+      <c r="U44" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V44" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W44" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X44" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D44,info!$C$11:$D$19), F44*100)</f>
+        <v>R4</v>
+      </c>
+      <c r="Y44" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z44" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-R4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>300</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3">
+        <v>400</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H45" s="3">
+        <v>5</v>
+      </c>
+      <c r="I45" s="4">
+        <v>7</v>
+      </c>
+      <c r="J45" s="4">
+        <v>1</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <v>30</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O45" s="3">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R45" s="3">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
+        <v>0</v>
+      </c>
+      <c r="T45" s="3">
+        <v>0</v>
+      </c>
+      <c r="U45" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V45" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W45" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X45" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D45,info!$C$11:$D$19), F45*100)</f>
+        <v>D4</v>
+      </c>
+      <c r="Y45" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z45" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-D4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>300</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3">
+        <v>400</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H46" s="3">
+        <v>5</v>
+      </c>
+      <c r="I46" s="4">
+        <v>7</v>
+      </c>
+      <c r="J46" s="4">
+        <v>1</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <v>30</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0</v>
+      </c>
+      <c r="P46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R46" s="3">
+        <v>0</v>
+      </c>
+      <c r="S46" s="3">
+        <v>0</v>
+      </c>
+      <c r="T46" s="3">
+        <v>0</v>
+      </c>
+      <c r="U46" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V46" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W46" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X46" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D46,info!$C$11:$D$19), F46*100)</f>
+        <v>R7</v>
+      </c>
+      <c r="Y46" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z46" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-R7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>300</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3">
+        <v>400</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H47" s="3">
+        <v>5</v>
+      </c>
+      <c r="I47" s="4">
+        <v>7</v>
+      </c>
+      <c r="J47" s="4">
+        <v>1</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
+        <v>30</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0</v>
+      </c>
+      <c r="P47" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R47" s="3">
+        <v>0</v>
+      </c>
+      <c r="S47" s="3">
+        <v>0</v>
+      </c>
+      <c r="T47" s="3">
+        <v>0</v>
+      </c>
+      <c r="U47" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V47" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W47" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X47" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D47,info!$C$11:$D$19), F47*100)</f>
+        <v>D7</v>
+      </c>
+      <c r="Y47" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M1</v>
+      </c>
+      <c r="Z47" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M1-T1-D7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>300</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3">
+        <v>400</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2</v>
+      </c>
+      <c r="F48" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H48" s="3">
+        <v>5</v>
+      </c>
+      <c r="I48" s="4">
+        <v>7</v>
+      </c>
+      <c r="J48" s="4">
+        <v>1</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <v>30</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R48" s="3">
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
+        <v>0</v>
+      </c>
+      <c r="T48" s="3">
+        <v>0</v>
+      </c>
+      <c r="U48" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V48" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W48" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X48" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D48,info!$C$11:$D$19), F48*100)</f>
+        <v>R7</v>
+      </c>
+      <c r="Y48" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-R7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>300</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3">
+        <v>400</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+      <c r="F49" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H49" s="3">
+        <v>5</v>
+      </c>
+      <c r="I49" s="4">
+        <v>7</v>
+      </c>
+      <c r="J49" s="4">
+        <v>1</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <v>30</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R49" s="3">
+        <v>0</v>
+      </c>
+      <c r="S49" s="3">
+        <v>0</v>
+      </c>
+      <c r="T49" s="3">
+        <v>0</v>
+      </c>
+      <c r="U49" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V49" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W49" s="3" t="str">
+        <f>AEP!$A$16</f>
+        <v>T1</v>
+      </c>
+      <c r="X49" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D49,info!$C$11:$D$19), F49*100)</f>
+        <v>D7</v>
+      </c>
+      <c r="Y49" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>M2</v>
+      </c>
+      <c r="Z49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>M2-T1-D7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add surv bias for tuneing purposes
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AEP" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="475">
   <si>
     <t>Trial</t>
   </si>
@@ -2741,11 +2741,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB393"/>
+  <dimension ref="A1:AB401"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K391" sqref="K391"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A382" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A394" sqref="A394:XFD394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37006,6 +37006,670 @@
         <v>M2-T9-D4</v>
       </c>
     </row>
+    <row r="394" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A394" s="3">
+        <v>300</v>
+      </c>
+      <c r="B394" s="3">
+        <v>0</v>
+      </c>
+      <c r="C394" s="3">
+        <v>400</v>
+      </c>
+      <c r="D394" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E394" s="3">
+        <v>2</v>
+      </c>
+      <c r="F394" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G394" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H394" s="3">
+        <v>5</v>
+      </c>
+      <c r="I394" s="4">
+        <v>7</v>
+      </c>
+      <c r="J394" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K394" s="3">
+        <v>0</v>
+      </c>
+      <c r="L394" s="3">
+        <v>30</v>
+      </c>
+      <c r="M394" s="3">
+        <v>0</v>
+      </c>
+      <c r="N394" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O394" s="3">
+        <v>0</v>
+      </c>
+      <c r="P394" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q394" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R394" s="3">
+        <v>0</v>
+      </c>
+      <c r="S394" s="3">
+        <v>0</v>
+      </c>
+      <c r="T394" s="3">
+        <v>0</v>
+      </c>
+      <c r="U394" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V394" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W394" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X394" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D394,info!$C$11:$D$19), F394*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y394" s="3" t="str">
+        <f t="shared" ref="Y394:Y401" si="15">IF(AND(B394=0,E394=1),"F1",IF(AND(B394=0,E394=2),"F2",IF(AND(B394=1,E394=1),"M1",IF(AND(B394=1,E394=2),"M2","?"))))</f>
+        <v>F2</v>
+      </c>
+      <c r="Z394" s="3" t="str">
+        <f t="shared" ref="Z394:Z401" si="16">CONCATENATE($Y394,"-",$W394,"-",$X394)</f>
+        <v>F2-T2-R1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A395" s="3">
+        <v>300</v>
+      </c>
+      <c r="B395" s="3">
+        <v>0</v>
+      </c>
+      <c r="C395" s="3">
+        <v>400</v>
+      </c>
+      <c r="D395" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E395" s="3">
+        <v>2</v>
+      </c>
+      <c r="F395" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G395" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H395" s="3">
+        <v>5</v>
+      </c>
+      <c r="I395" s="4">
+        <v>7</v>
+      </c>
+      <c r="J395" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K395" s="3">
+        <v>0</v>
+      </c>
+      <c r="L395" s="3">
+        <v>30</v>
+      </c>
+      <c r="M395" s="3">
+        <v>0</v>
+      </c>
+      <c r="N395" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O395" s="3">
+        <v>0</v>
+      </c>
+      <c r="P395" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q395" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R395" s="3">
+        <v>0</v>
+      </c>
+      <c r="S395" s="3">
+        <v>0</v>
+      </c>
+      <c r="T395" s="3">
+        <v>0</v>
+      </c>
+      <c r="U395" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V395" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W395" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X395" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D395,info!$C$11:$D$19), F395*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y395" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>F2</v>
+      </c>
+      <c r="Z395" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>F2-T2-D1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A396" s="3">
+        <v>300</v>
+      </c>
+      <c r="B396" s="3">
+        <v>1</v>
+      </c>
+      <c r="C396" s="3">
+        <v>400</v>
+      </c>
+      <c r="D396" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E396" s="3">
+        <v>2</v>
+      </c>
+      <c r="F396" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G396" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H396" s="3">
+        <v>5</v>
+      </c>
+      <c r="I396" s="4">
+        <v>7</v>
+      </c>
+      <c r="J396" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K396" s="3">
+        <v>0</v>
+      </c>
+      <c r="L396" s="3">
+        <v>30</v>
+      </c>
+      <c r="M396" s="3">
+        <v>0</v>
+      </c>
+      <c r="N396" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O396" s="3">
+        <v>0</v>
+      </c>
+      <c r="P396" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q396" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R396" s="3">
+        <v>0</v>
+      </c>
+      <c r="S396" s="3">
+        <v>0</v>
+      </c>
+      <c r="T396" s="3">
+        <v>0</v>
+      </c>
+      <c r="U396" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V396" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W396" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X396" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D396,info!$C$11:$D$19), F396*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y396" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>M2</v>
+      </c>
+      <c r="Z396" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>M2-T2-R1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A397" s="3">
+        <v>300</v>
+      </c>
+      <c r="B397" s="3">
+        <v>1</v>
+      </c>
+      <c r="C397" s="3">
+        <v>400</v>
+      </c>
+      <c r="D397" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E397" s="3">
+        <v>2</v>
+      </c>
+      <c r="F397" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G397" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H397" s="3">
+        <v>5</v>
+      </c>
+      <c r="I397" s="4">
+        <v>7</v>
+      </c>
+      <c r="J397" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K397" s="3">
+        <v>0</v>
+      </c>
+      <c r="L397" s="3">
+        <v>30</v>
+      </c>
+      <c r="M397" s="3">
+        <v>0</v>
+      </c>
+      <c r="N397" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O397" s="3">
+        <v>0</v>
+      </c>
+      <c r="P397" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q397" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R397" s="3">
+        <v>0</v>
+      </c>
+      <c r="S397" s="3">
+        <v>0</v>
+      </c>
+      <c r="T397" s="3">
+        <v>0</v>
+      </c>
+      <c r="U397" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V397" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W397" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X397" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D397,info!$C$11:$D$19), F397*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y397" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>M2</v>
+      </c>
+      <c r="Z397" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>M2-T2-D1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A398" s="3">
+        <v>300</v>
+      </c>
+      <c r="B398" s="3">
+        <v>0</v>
+      </c>
+      <c r="C398" s="3">
+        <v>400</v>
+      </c>
+      <c r="D398" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E398" s="3">
+        <v>2</v>
+      </c>
+      <c r="F398" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G398" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H398" s="3">
+        <v>5</v>
+      </c>
+      <c r="I398" s="4">
+        <v>7</v>
+      </c>
+      <c r="J398" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K398" s="3">
+        <v>0</v>
+      </c>
+      <c r="L398" s="3">
+        <v>30</v>
+      </c>
+      <c r="M398" s="3">
+        <v>0</v>
+      </c>
+      <c r="N398" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O398" s="3">
+        <v>0</v>
+      </c>
+      <c r="P398" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q398" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R398" s="3">
+        <v>0</v>
+      </c>
+      <c r="S398" s="3">
+        <v>0</v>
+      </c>
+      <c r="T398" s="3">
+        <v>0</v>
+      </c>
+      <c r="U398" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V398" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W398" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X398" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D398,info!$C$11:$D$19), F398*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y398" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>F2</v>
+      </c>
+      <c r="Z398" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>F2-T3-R1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A399" s="3">
+        <v>300</v>
+      </c>
+      <c r="B399" s="3">
+        <v>0</v>
+      </c>
+      <c r="C399" s="3">
+        <v>400</v>
+      </c>
+      <c r="D399" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E399" s="3">
+        <v>2</v>
+      </c>
+      <c r="F399" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G399" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H399" s="3">
+        <v>5</v>
+      </c>
+      <c r="I399" s="4">
+        <v>7</v>
+      </c>
+      <c r="J399" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K399" s="3">
+        <v>0</v>
+      </c>
+      <c r="L399" s="3">
+        <v>30</v>
+      </c>
+      <c r="M399" s="3">
+        <v>0</v>
+      </c>
+      <c r="N399" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O399" s="3">
+        <v>0</v>
+      </c>
+      <c r="P399" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q399" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R399" s="3">
+        <v>0</v>
+      </c>
+      <c r="S399" s="3">
+        <v>0</v>
+      </c>
+      <c r="T399" s="3">
+        <v>0</v>
+      </c>
+      <c r="U399" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V399" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W399" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X399" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D399,info!$C$11:$D$19), F399*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y399" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>F2</v>
+      </c>
+      <c r="Z399" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>F2-T3-D1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A400" s="3">
+        <v>300</v>
+      </c>
+      <c r="B400" s="3">
+        <v>1</v>
+      </c>
+      <c r="C400" s="3">
+        <v>400</v>
+      </c>
+      <c r="D400" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E400" s="3">
+        <v>2</v>
+      </c>
+      <c r="F400" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G400" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H400" s="3">
+        <v>5</v>
+      </c>
+      <c r="I400" s="4">
+        <v>7</v>
+      </c>
+      <c r="J400" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K400" s="3">
+        <v>0</v>
+      </c>
+      <c r="L400" s="3">
+        <v>30</v>
+      </c>
+      <c r="M400" s="3">
+        <v>0</v>
+      </c>
+      <c r="N400" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O400" s="3">
+        <v>0</v>
+      </c>
+      <c r="P400" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q400" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R400" s="3">
+        <v>0</v>
+      </c>
+      <c r="S400" s="3">
+        <v>0</v>
+      </c>
+      <c r="T400" s="3">
+        <v>0</v>
+      </c>
+      <c r="U400" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V400" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W400" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X400" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D400,info!$C$11:$D$19), F400*100)</f>
+        <v>R1</v>
+      </c>
+      <c r="Y400" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>M2</v>
+      </c>
+      <c r="Z400" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>M2-T3-R1</v>
+      </c>
+    </row>
+    <row r="401" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A401" s="3">
+        <v>300</v>
+      </c>
+      <c r="B401" s="3">
+        <v>1</v>
+      </c>
+      <c r="C401" s="3">
+        <v>400</v>
+      </c>
+      <c r="D401" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E401" s="3">
+        <v>2</v>
+      </c>
+      <c r="F401" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G401" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H401" s="3">
+        <v>5</v>
+      </c>
+      <c r="I401" s="4">
+        <v>7</v>
+      </c>
+      <c r="J401" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K401" s="3">
+        <v>0</v>
+      </c>
+      <c r="L401" s="3">
+        <v>30</v>
+      </c>
+      <c r="M401" s="3">
+        <v>0</v>
+      </c>
+      <c r="N401" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O401" s="3">
+        <v>0</v>
+      </c>
+      <c r="P401" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q401" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R401" s="3">
+        <v>0</v>
+      </c>
+      <c r="S401" s="3">
+        <v>0</v>
+      </c>
+      <c r="T401" s="3">
+        <v>0</v>
+      </c>
+      <c r="U401" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V401" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W401" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X401" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D401,info!$C$11:$D$19), F401*100)</f>
+        <v>D1</v>
+      </c>
+      <c r="Y401" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>M2</v>
+      </c>
+      <c r="Z401" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>M2-T3-D1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB393"/>
   <sortState ref="A34:I45">
@@ -37022,7 +37686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA25" sqref="AA25"/>
     </sheetView>

</xml_diff>

<commit_message>
Remove Natural mortality trials from tune
</commit_message>
<xml_diff>
--- a/Trials_KFJ.xlsx
+++ b/Trials_KFJ.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18210" windowHeight="10215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AEP" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="475">
   <si>
     <t>Trial</t>
   </si>
@@ -2741,11 +2741,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB401"/>
+  <dimension ref="A1:AB402"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A382" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A394" sqref="A394:XFD394"/>
+      <selection pane="bottomLeft" activeCell="K404" sqref="K404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37081,11 +37081,11 @@
         <v>R1</v>
       </c>
       <c r="Y394" s="3" t="str">
-        <f t="shared" ref="Y394:Y401" si="15">IF(AND(B394=0,E394=1),"F1",IF(AND(B394=0,E394=2),"F2",IF(AND(B394=1,E394=1),"M1",IF(AND(B394=1,E394=2),"M2","?"))))</f>
+        <f t="shared" ref="Y394:Y402" si="15">IF(AND(B394=0,E394=1),"F1",IF(AND(B394=0,E394=2),"F2",IF(AND(B394=1,E394=1),"M1",IF(AND(B394=1,E394=2),"M2","?"))))</f>
         <v>F2</v>
       </c>
       <c r="Z394" s="3" t="str">
-        <f t="shared" ref="Z394:Z401" si="16">CONCATENATE($Y394,"-",$W394,"-",$X394)</f>
+        <f t="shared" ref="Z394:Z402" si="16">CONCATENATE($Y394,"-",$W394,"-",$X394)</f>
         <v>F2-T2-R1</v>
       </c>
     </row>
@@ -37668,6 +37668,89 @@
       <c r="Z401" s="3" t="str">
         <f t="shared" si="16"/>
         <v>M2-T3-D1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A402" s="3">
+        <v>300</v>
+      </c>
+      <c r="B402" s="3">
+        <v>0</v>
+      </c>
+      <c r="C402" s="3">
+        <v>400</v>
+      </c>
+      <c r="D402" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E402" s="3">
+        <v>2</v>
+      </c>
+      <c r="F402" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G402" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H402" s="3">
+        <v>5</v>
+      </c>
+      <c r="I402" s="4">
+        <v>7</v>
+      </c>
+      <c r="J402" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K402" s="3">
+        <v>0</v>
+      </c>
+      <c r="L402" s="3">
+        <v>30</v>
+      </c>
+      <c r="M402" s="3">
+        <v>0</v>
+      </c>
+      <c r="N402" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O402" s="3">
+        <v>0</v>
+      </c>
+      <c r="P402" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q402" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="R402" s="3">
+        <v>0</v>
+      </c>
+      <c r="S402" s="3">
+        <v>0</v>
+      </c>
+      <c r="T402" s="3">
+        <v>0</v>
+      </c>
+      <c r="U402" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V402" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="W402" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X402" s="3" t="str">
+        <f>CONCATENATE(LOOKUP(D402,info!$C$11:$D$19), F402*100)</f>
+        <v>S1</v>
+      </c>
+      <c r="Y402" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>F2</v>
+      </c>
+      <c r="Z402" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>F2-T3-S1</v>
       </c>
     </row>
   </sheetData>
@@ -37684,11 +37767,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA25" sqref="AA25"/>
+      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39819,2022 +39902,6 @@
         <v>F2-T1-D7</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>300</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>400</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H26" s="3">
-        <v>5</v>
-      </c>
-      <c r="I26" s="4">
-        <v>7</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="K26" s="3">
-        <v>0</v>
-      </c>
-      <c r="L26" s="3">
-        <v>30</v>
-      </c>
-      <c r="M26" s="3">
-        <v>0</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O26" s="3">
-        <v>0</v>
-      </c>
-      <c r="P26" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R26" s="3">
-        <v>0</v>
-      </c>
-      <c r="S26" s="3">
-        <v>0</v>
-      </c>
-      <c r="T26" s="3">
-        <v>0</v>
-      </c>
-      <c r="U26" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V26" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W26" s="3" t="str">
-        <f>AEP!$A$17</f>
-        <v>T2</v>
-      </c>
-      <c r="X26" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D26,info!$C$11:$D$19), F26*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y26" s="3" t="str">
-        <f t="shared" ref="Y26:Y49" si="2">IF(AND(B26=0,E26=1),"F1",IF(AND(B26=0,E26=2),"F2",IF(AND(B26=1,E26=1),"M1",IF(AND(B26=1,E26=2),"M2","?"))))</f>
-        <v>M1</v>
-      </c>
-      <c r="Z26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T2-R1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>300</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3">
-        <v>400</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H27" s="3">
-        <v>5</v>
-      </c>
-      <c r="I27" s="4">
-        <v>7</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="K27" s="3">
-        <v>0</v>
-      </c>
-      <c r="L27" s="3">
-        <v>30</v>
-      </c>
-      <c r="M27" s="3">
-        <v>0</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O27" s="3">
-        <v>0</v>
-      </c>
-      <c r="P27" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R27" s="3">
-        <v>0</v>
-      </c>
-      <c r="S27" s="3">
-        <v>0</v>
-      </c>
-      <c r="T27" s="3">
-        <v>0</v>
-      </c>
-      <c r="U27" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V27" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W27" s="3" t="str">
-        <f>AEP!$A$17</f>
-        <v>T2</v>
-      </c>
-      <c r="X27" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D27,info!$C$11:$D$19), F27*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y27" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T2-D1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>300</v>
-      </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3">
-        <v>400</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E28" s="3">
-        <v>2</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H28" s="3">
-        <v>5</v>
-      </c>
-      <c r="I28" s="4">
-        <v>7</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
-      <c r="L28" s="3">
-        <v>30</v>
-      </c>
-      <c r="M28" s="3">
-        <v>0</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0</v>
-      </c>
-      <c r="P28" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R28" s="3">
-        <v>0</v>
-      </c>
-      <c r="S28" s="3">
-        <v>0</v>
-      </c>
-      <c r="T28" s="3">
-        <v>0</v>
-      </c>
-      <c r="U28" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V28" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W28" s="3" t="str">
-        <f>AEP!$A$17</f>
-        <v>T2</v>
-      </c>
-      <c r="X28" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D28,info!$C$11:$D$19), F28*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y28" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T2-R1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>300</v>
-      </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3">
-        <v>400</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E29" s="3">
-        <v>2</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H29" s="3">
-        <v>5</v>
-      </c>
-      <c r="I29" s="4">
-        <v>7</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="K29" s="3">
-        <v>0</v>
-      </c>
-      <c r="L29" s="3">
-        <v>30</v>
-      </c>
-      <c r="M29" s="3">
-        <v>0</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O29" s="3">
-        <v>0</v>
-      </c>
-      <c r="P29" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R29" s="3">
-        <v>0</v>
-      </c>
-      <c r="S29" s="3">
-        <v>0</v>
-      </c>
-      <c r="T29" s="3">
-        <v>0</v>
-      </c>
-      <c r="U29" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V29" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W29" s="3" t="str">
-        <f>AEP!$A$17</f>
-        <v>T2</v>
-      </c>
-      <c r="X29" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D29,info!$C$11:$D$19), F29*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y29" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T2-D1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>300</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3">
-        <v>400</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H30" s="3">
-        <v>5</v>
-      </c>
-      <c r="I30" s="4">
-        <v>7</v>
-      </c>
-      <c r="J30" s="4">
-        <v>1</v>
-      </c>
-      <c r="K30" s="3">
-        <v>0</v>
-      </c>
-      <c r="L30" s="3">
-        <v>30</v>
-      </c>
-      <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O30" s="3">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R30" s="3">
-        <v>0</v>
-      </c>
-      <c r="S30" s="3">
-        <v>0</v>
-      </c>
-      <c r="T30" s="3">
-        <v>0</v>
-      </c>
-      <c r="U30" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V30" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W30" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X30" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D30,info!$C$11:$D$19), F30*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y30" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-R1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>300</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>400</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H31" s="3">
-        <v>5</v>
-      </c>
-      <c r="I31" s="4">
-        <v>7</v>
-      </c>
-      <c r="J31" s="4">
-        <v>1</v>
-      </c>
-      <c r="K31" s="3">
-        <v>0</v>
-      </c>
-      <c r="L31" s="3">
-        <v>30</v>
-      </c>
-      <c r="M31" s="3">
-        <v>0</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O31" s="3">
-        <v>0</v>
-      </c>
-      <c r="P31" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R31" s="3">
-        <v>0</v>
-      </c>
-      <c r="S31" s="3">
-        <v>0</v>
-      </c>
-      <c r="T31" s="3">
-        <v>0</v>
-      </c>
-      <c r="U31" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V31" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W31" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X31" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D31,info!$C$11:$D$19), F31*100)</f>
-        <v>S1</v>
-      </c>
-      <c r="Y31" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-S1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>300</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>400</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>5</v>
-      </c>
-      <c r="I32" s="4">
-        <v>7</v>
-      </c>
-      <c r="J32" s="4">
-        <v>1</v>
-      </c>
-      <c r="K32" s="3">
-        <v>0</v>
-      </c>
-      <c r="L32" s="3">
-        <v>30</v>
-      </c>
-      <c r="M32" s="3">
-        <v>0</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O32" s="3">
-        <v>0</v>
-      </c>
-      <c r="P32" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R32" s="3">
-        <v>0</v>
-      </c>
-      <c r="S32" s="3">
-        <v>0</v>
-      </c>
-      <c r="T32" s="3">
-        <v>0</v>
-      </c>
-      <c r="U32" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V32" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W32" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X32" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D32,info!$C$11:$D$19), F32*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y32" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-D1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>300</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>400</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E33" s="3">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H33" s="3">
-        <v>5</v>
-      </c>
-      <c r="I33" s="4">
-        <v>7</v>
-      </c>
-      <c r="J33" s="4">
-        <v>1</v>
-      </c>
-      <c r="K33" s="3">
-        <v>0</v>
-      </c>
-      <c r="L33" s="3">
-        <v>30</v>
-      </c>
-      <c r="M33" s="3">
-        <v>0</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O33" s="3">
-        <v>0</v>
-      </c>
-      <c r="P33" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R33" s="3">
-        <v>0</v>
-      </c>
-      <c r="S33" s="3">
-        <v>0</v>
-      </c>
-      <c r="T33" s="3">
-        <v>0</v>
-      </c>
-      <c r="U33" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V33" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W33" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X33" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D33,info!$C$11:$D$19), F33*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y33" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-R1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>300</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>400</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E34" s="3">
-        <v>2</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H34" s="3">
-        <v>5</v>
-      </c>
-      <c r="I34" s="4">
-        <v>7</v>
-      </c>
-      <c r="J34" s="4">
-        <v>1</v>
-      </c>
-      <c r="K34" s="3">
-        <v>0</v>
-      </c>
-      <c r="L34" s="3">
-        <v>30</v>
-      </c>
-      <c r="M34" s="3">
-        <v>0</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O34" s="3">
-        <v>0</v>
-      </c>
-      <c r="P34" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R34" s="3">
-        <v>0</v>
-      </c>
-      <c r="S34" s="3">
-        <v>0</v>
-      </c>
-      <c r="T34" s="3">
-        <v>0</v>
-      </c>
-      <c r="U34" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V34" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W34" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X34" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D34,info!$C$11:$D$19), F34*100)</f>
-        <v>S1</v>
-      </c>
-      <c r="Y34" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-S1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>300</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3">
-        <v>400</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E35" s="3">
-        <v>2</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H35" s="3">
-        <v>5</v>
-      </c>
-      <c r="I35" s="4">
-        <v>7</v>
-      </c>
-      <c r="J35" s="4">
-        <v>1</v>
-      </c>
-      <c r="K35" s="3">
-        <v>0</v>
-      </c>
-      <c r="L35" s="3">
-        <v>30</v>
-      </c>
-      <c r="M35" s="3">
-        <v>0</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O35" s="3">
-        <v>0</v>
-      </c>
-      <c r="P35" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R35" s="3">
-        <v>0</v>
-      </c>
-      <c r="S35" s="3">
-        <v>0</v>
-      </c>
-      <c r="T35" s="3">
-        <v>0</v>
-      </c>
-      <c r="U35" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V35" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W35" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X35" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D35,info!$C$11:$D$19), F35*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y35" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-D1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>300</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3">
-        <v>400</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H36" s="3">
-        <v>5</v>
-      </c>
-      <c r="I36" s="4">
-        <v>7</v>
-      </c>
-      <c r="J36" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K36" s="3">
-        <v>0</v>
-      </c>
-      <c r="L36" s="3">
-        <v>30</v>
-      </c>
-      <c r="M36" s="3">
-        <v>0</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O36" s="3">
-        <v>0</v>
-      </c>
-      <c r="P36" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R36" s="3">
-        <v>0</v>
-      </c>
-      <c r="S36" s="3">
-        <v>0</v>
-      </c>
-      <c r="T36" s="3">
-        <v>0</v>
-      </c>
-      <c r="U36" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V36" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W36" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X36" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D36,info!$C$11:$D$19), F36*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T3-R1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>300</v>
-      </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3">
-        <v>400</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E37" s="3">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H37" s="3">
-        <v>5</v>
-      </c>
-      <c r="I37" s="4">
-        <v>7</v>
-      </c>
-      <c r="J37" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K37" s="3">
-        <v>0</v>
-      </c>
-      <c r="L37" s="3">
-        <v>30</v>
-      </c>
-      <c r="M37" s="3">
-        <v>0</v>
-      </c>
-      <c r="N37" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O37" s="3">
-        <v>0</v>
-      </c>
-      <c r="P37" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R37" s="3">
-        <v>0</v>
-      </c>
-      <c r="S37" s="3">
-        <v>0</v>
-      </c>
-      <c r="T37" s="3">
-        <v>0</v>
-      </c>
-      <c r="U37" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V37" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W37" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X37" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D37,info!$C$11:$D$19), F37*100)</f>
-        <v>S1</v>
-      </c>
-      <c r="Y37" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T3-S1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>300</v>
-      </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3">
-        <v>400</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H38" s="3">
-        <v>5</v>
-      </c>
-      <c r="I38" s="4">
-        <v>7</v>
-      </c>
-      <c r="J38" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0</v>
-      </c>
-      <c r="L38" s="3">
-        <v>30</v>
-      </c>
-      <c r="M38" s="3">
-        <v>0</v>
-      </c>
-      <c r="N38" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O38" s="3">
-        <v>0</v>
-      </c>
-      <c r="P38" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R38" s="3">
-        <v>0</v>
-      </c>
-      <c r="S38" s="3">
-        <v>0</v>
-      </c>
-      <c r="T38" s="3">
-        <v>0</v>
-      </c>
-      <c r="U38" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V38" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W38" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X38" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D38,info!$C$11:$D$19), F38*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y38" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T3-D1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>300</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3">
-        <v>400</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H39" s="3">
-        <v>5</v>
-      </c>
-      <c r="I39" s="4">
-        <v>7</v>
-      </c>
-      <c r="J39" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K39" s="3">
-        <v>0</v>
-      </c>
-      <c r="L39" s="3">
-        <v>30</v>
-      </c>
-      <c r="M39" s="3">
-        <v>0</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O39" s="3">
-        <v>0</v>
-      </c>
-      <c r="P39" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R39" s="3">
-        <v>0</v>
-      </c>
-      <c r="S39" s="3">
-        <v>0</v>
-      </c>
-      <c r="T39" s="3">
-        <v>0</v>
-      </c>
-      <c r="U39" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V39" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W39" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X39" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D39,info!$C$11:$D$19), F39*100)</f>
-        <v>R1</v>
-      </c>
-      <c r="Y39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z39" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T3-R1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>300</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
-      <c r="C40" s="3">
-        <v>400</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E40" s="3">
-        <v>2</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H40" s="3">
-        <v>5</v>
-      </c>
-      <c r="I40" s="4">
-        <v>7</v>
-      </c>
-      <c r="J40" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K40" s="3">
-        <v>0</v>
-      </c>
-      <c r="L40" s="3">
-        <v>30</v>
-      </c>
-      <c r="M40" s="3">
-        <v>0</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0</v>
-      </c>
-      <c r="P40" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R40" s="3">
-        <v>0</v>
-      </c>
-      <c r="S40" s="3">
-        <v>0</v>
-      </c>
-      <c r="T40" s="3">
-        <v>0</v>
-      </c>
-      <c r="U40" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V40" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W40" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X40" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D40,info!$C$11:$D$19), F40*100)</f>
-        <v>S1</v>
-      </c>
-      <c r="Y40" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z40" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T3-S1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>300</v>
-      </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3">
-        <v>400</v>
-      </c>
-      <c r="D41" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E41" s="3">
-        <v>2</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H41" s="3">
-        <v>5</v>
-      </c>
-      <c r="I41" s="4">
-        <v>7</v>
-      </c>
-      <c r="J41" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="K41" s="3">
-        <v>0</v>
-      </c>
-      <c r="L41" s="3">
-        <v>30</v>
-      </c>
-      <c r="M41" s="3">
-        <v>0</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O41" s="3">
-        <v>0</v>
-      </c>
-      <c r="P41" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R41" s="3">
-        <v>0</v>
-      </c>
-      <c r="S41" s="3">
-        <v>0</v>
-      </c>
-      <c r="T41" s="3">
-        <v>0</v>
-      </c>
-      <c r="U41" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V41" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W41" s="3" t="str">
-        <f>AEP!$A$18</f>
-        <v>T3</v>
-      </c>
-      <c r="X41" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D41,info!$C$11:$D$19), F41*100)</f>
-        <v>D1</v>
-      </c>
-      <c r="Y41" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T3-D1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>300</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3">
-        <v>400</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E42" s="3">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="G42" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H42" s="3">
-        <v>5</v>
-      </c>
-      <c r="I42" s="4">
-        <v>7</v>
-      </c>
-      <c r="J42" s="4">
-        <v>1</v>
-      </c>
-      <c r="K42" s="3">
-        <v>0</v>
-      </c>
-      <c r="L42" s="3">
-        <v>30</v>
-      </c>
-      <c r="M42" s="3">
-        <v>0</v>
-      </c>
-      <c r="N42" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O42" s="3">
-        <v>0</v>
-      </c>
-      <c r="P42" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R42" s="3">
-        <v>0</v>
-      </c>
-      <c r="S42" s="3">
-        <v>0</v>
-      </c>
-      <c r="T42" s="3">
-        <v>0</v>
-      </c>
-      <c r="U42" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V42" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W42" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X42" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D42,info!$C$11:$D$19), F42*100)</f>
-        <v>R4</v>
-      </c>
-      <c r="Y42" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z42" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-R4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>300</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3">
-        <v>400</v>
-      </c>
-      <c r="D43" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="G43" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H43" s="3">
-        <v>5</v>
-      </c>
-      <c r="I43" s="4">
-        <v>7</v>
-      </c>
-      <c r="J43" s="4">
-        <v>1</v>
-      </c>
-      <c r="K43" s="3">
-        <v>0</v>
-      </c>
-      <c r="L43" s="3">
-        <v>30</v>
-      </c>
-      <c r="M43" s="3">
-        <v>0</v>
-      </c>
-      <c r="N43" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O43" s="3">
-        <v>0</v>
-      </c>
-      <c r="P43" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R43" s="3">
-        <v>0</v>
-      </c>
-      <c r="S43" s="3">
-        <v>0</v>
-      </c>
-      <c r="T43" s="3">
-        <v>0</v>
-      </c>
-      <c r="U43" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V43" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W43" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X43" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D43,info!$C$11:$D$19), F43*100)</f>
-        <v>D4</v>
-      </c>
-      <c r="Y43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-D4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>300</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3">
-        <v>400</v>
-      </c>
-      <c r="D44" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E44" s="3">
-        <v>2</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="G44" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H44" s="3">
-        <v>5</v>
-      </c>
-      <c r="I44" s="4">
-        <v>7</v>
-      </c>
-      <c r="J44" s="4">
-        <v>1</v>
-      </c>
-      <c r="K44" s="3">
-        <v>0</v>
-      </c>
-      <c r="L44" s="3">
-        <v>30</v>
-      </c>
-      <c r="M44" s="3">
-        <v>0</v>
-      </c>
-      <c r="N44" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O44" s="3">
-        <v>0</v>
-      </c>
-      <c r="P44" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R44" s="3">
-        <v>0</v>
-      </c>
-      <c r="S44" s="3">
-        <v>0</v>
-      </c>
-      <c r="T44" s="3">
-        <v>0</v>
-      </c>
-      <c r="U44" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V44" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W44" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X44" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D44,info!$C$11:$D$19), F44*100)</f>
-        <v>R4</v>
-      </c>
-      <c r="Y44" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-R4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>300</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3">
-        <v>400</v>
-      </c>
-      <c r="D45" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E45" s="3">
-        <v>2</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="G45" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H45" s="3">
-        <v>5</v>
-      </c>
-      <c r="I45" s="4">
-        <v>7</v>
-      </c>
-      <c r="J45" s="4">
-        <v>1</v>
-      </c>
-      <c r="K45" s="3">
-        <v>0</v>
-      </c>
-      <c r="L45" s="3">
-        <v>30</v>
-      </c>
-      <c r="M45" s="3">
-        <v>0</v>
-      </c>
-      <c r="N45" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O45" s="3">
-        <v>0</v>
-      </c>
-      <c r="P45" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R45" s="3">
-        <v>0</v>
-      </c>
-      <c r="S45" s="3">
-        <v>0</v>
-      </c>
-      <c r="T45" s="3">
-        <v>0</v>
-      </c>
-      <c r="U45" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V45" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W45" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X45" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D45,info!$C$11:$D$19), F45*100)</f>
-        <v>D4</v>
-      </c>
-      <c r="Y45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-D4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>300</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3">
-        <v>400</v>
-      </c>
-      <c r="D46" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H46" s="3">
-        <v>5</v>
-      </c>
-      <c r="I46" s="4">
-        <v>7</v>
-      </c>
-      <c r="J46" s="4">
-        <v>1</v>
-      </c>
-      <c r="K46" s="3">
-        <v>0</v>
-      </c>
-      <c r="L46" s="3">
-        <v>30</v>
-      </c>
-      <c r="M46" s="3">
-        <v>0</v>
-      </c>
-      <c r="N46" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O46" s="3">
-        <v>0</v>
-      </c>
-      <c r="P46" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R46" s="3">
-        <v>0</v>
-      </c>
-      <c r="S46" s="3">
-        <v>0</v>
-      </c>
-      <c r="T46" s="3">
-        <v>0</v>
-      </c>
-      <c r="U46" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V46" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W46" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X46" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D46,info!$C$11:$D$19), F46*100)</f>
-        <v>R7</v>
-      </c>
-      <c r="Y46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-R7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>300</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3">
-        <v>400</v>
-      </c>
-      <c r="D47" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H47" s="3">
-        <v>5</v>
-      </c>
-      <c r="I47" s="4">
-        <v>7</v>
-      </c>
-      <c r="J47" s="4">
-        <v>1</v>
-      </c>
-      <c r="K47" s="3">
-        <v>0</v>
-      </c>
-      <c r="L47" s="3">
-        <v>30</v>
-      </c>
-      <c r="M47" s="3">
-        <v>0</v>
-      </c>
-      <c r="N47" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O47" s="3">
-        <v>0</v>
-      </c>
-      <c r="P47" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R47" s="3">
-        <v>0</v>
-      </c>
-      <c r="S47" s="3">
-        <v>0</v>
-      </c>
-      <c r="T47" s="3">
-        <v>0</v>
-      </c>
-      <c r="U47" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V47" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W47" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X47" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D47,info!$C$11:$D$19), F47*100)</f>
-        <v>D7</v>
-      </c>
-      <c r="Y47" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M1</v>
-      </c>
-      <c r="Z47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M1-T1-D7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>300</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3">
-        <v>400</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2</v>
-      </c>
-      <c r="F48" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G48" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H48" s="3">
-        <v>5</v>
-      </c>
-      <c r="I48" s="4">
-        <v>7</v>
-      </c>
-      <c r="J48" s="4">
-        <v>1</v>
-      </c>
-      <c r="K48" s="3">
-        <v>0</v>
-      </c>
-      <c r="L48" s="3">
-        <v>30</v>
-      </c>
-      <c r="M48" s="3">
-        <v>0</v>
-      </c>
-      <c r="N48" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O48" s="3">
-        <v>0</v>
-      </c>
-      <c r="P48" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R48" s="3">
-        <v>0</v>
-      </c>
-      <c r="S48" s="3">
-        <v>0</v>
-      </c>
-      <c r="T48" s="3">
-        <v>0</v>
-      </c>
-      <c r="U48" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V48" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W48" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X48" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D48,info!$C$11:$D$19), F48*100)</f>
-        <v>R7</v>
-      </c>
-      <c r="Y48" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-R7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>300</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-      <c r="C49" s="3">
-        <v>400</v>
-      </c>
-      <c r="D49" s="4">
-        <v>0.99</v>
-      </c>
-      <c r="E49" s="3">
-        <v>2</v>
-      </c>
-      <c r="F49" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G49" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H49" s="3">
-        <v>5</v>
-      </c>
-      <c r="I49" s="4">
-        <v>7</v>
-      </c>
-      <c r="J49" s="4">
-        <v>1</v>
-      </c>
-      <c r="K49" s="3">
-        <v>0</v>
-      </c>
-      <c r="L49" s="3">
-        <v>30</v>
-      </c>
-      <c r="M49" s="3">
-        <v>0</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="O49" s="3">
-        <v>0</v>
-      </c>
-      <c r="P49" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="R49" s="3">
-        <v>0</v>
-      </c>
-      <c r="S49" s="3">
-        <v>0</v>
-      </c>
-      <c r="T49" s="3">
-        <v>0</v>
-      </c>
-      <c r="U49" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="V49" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="W49" s="3" t="str">
-        <f>AEP!$A$16</f>
-        <v>T1</v>
-      </c>
-      <c r="X49" s="3" t="str">
-        <f>CONCATENATE(LOOKUP(D49,info!$C$11:$D$19), F49*100)</f>
-        <v>D7</v>
-      </c>
-      <c r="Y49" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>M2</v>
-      </c>
-      <c r="Z49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>M2-T1-D7</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:AA23"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>